<commit_message>
Object with key-value pairs from excel ready to populate XML
</commit_message>
<xml_diff>
--- a/template_v1.xlsx
+++ b/template_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64A7D62C-9F7E-884D-85EA-876D1CA7D2B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0779E1D-DC4D-7642-96F2-5CB9045F5D33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7600" yWindow="460" windowWidth="26000" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="122">
   <si>
     <t>Yes</t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t>Di-Ammonium Phosphate</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1027,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1090,6 +1093,9 @@
     <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>72</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Combine data with sample data ready
</commit_message>
<xml_diff>
--- a/template_v1.xlsx
+++ b/template_v1.xlsx
@@ -8,25 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7828D0A1-7C38-9D40-BD0A-34F3AC339079}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EBC989-FCA8-7D4A-A30F-8010A512DEFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="460" windowWidth="26000" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
+    <workbookView xWindow="6980" yWindow="460" windowWidth="26620" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
-    <sheet name="pre1980" sheetId="6" r:id="rId2"/>
-    <sheet name="yr80" sheetId="7" r:id="rId3"/>
-    <sheet name="yesno" sheetId="2" r:id="rId4"/>
-    <sheet name="crops" sheetId="3" r:id="rId5"/>
-    <sheet name="covercrops" sheetId="4" r:id="rId6"/>
-    <sheet name="treesvines" sheetId="5" r:id="rId7"/>
-    <sheet name="binary" sheetId="9" r:id="rId8"/>
-    <sheet name="tillagetype" sheetId="10" r:id="rId9"/>
-    <sheet name="napplicationtype" sheetId="11" r:id="rId10"/>
-    <sheet name="tillage" sheetId="8" r:id="rId11"/>
+    <sheet name="eep" sheetId="13" r:id="rId2"/>
+    <sheet name="pre1980" sheetId="6" r:id="rId3"/>
+    <sheet name="yr80" sheetId="7" r:id="rId4"/>
+    <sheet name="yesno" sheetId="2" r:id="rId5"/>
+    <sheet name="crops" sheetId="3" r:id="rId6"/>
+    <sheet name="covercrops" sheetId="4" r:id="rId7"/>
+    <sheet name="treesvines" sheetId="5" r:id="rId8"/>
+    <sheet name="binary" sheetId="9" r:id="rId9"/>
+    <sheet name="tillagetype" sheetId="10" r:id="rId10"/>
+    <sheet name="napplicationtype" sheetId="11" r:id="rId11"/>
+    <sheet name="napplicationmethod" sheetId="12" r:id="rId12"/>
+    <sheet name="tillage" sheetId="8" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="Crops">[1]Units!$A$2:$A$34</definedName>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="138">
   <si>
     <t>Yes</t>
   </si>
@@ -412,44 +414,62 @@
     <t>Di-Ammonium Phosphate</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>amount of fertilizer</t>
-  </si>
-  <si>
-    <t>organic fertilizer</t>
-  </si>
-  <si>
-    <t>ranges for numeric value</t>
-  </si>
-  <si>
-    <t>vary depend on crop</t>
-  </si>
-  <si>
-    <t>NApplicationMethod</t>
-  </si>
-  <si>
-    <t>….</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>POLYGON((-123.12342 31.2009), (-121.334 32.333))</t>
-  </si>
-  <si>
     <t>AREA</t>
   </si>
   <si>
     <t>SRID</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>CRPType</t>
+  </si>
+  <si>
+    <t>Surface Broadcast</t>
+  </si>
+  <si>
+    <t>Surface Band / Sidedress</t>
+  </si>
+  <si>
+    <t>Incorporate / Inject</t>
+  </si>
+  <si>
+    <t>Fertigation</t>
+  </si>
+  <si>
+    <t>Aerial Application</t>
+  </si>
+  <si>
+    <t>n_application_method</t>
+  </si>
+  <si>
+    <t>n_application_amount</t>
+  </si>
+  <si>
+    <t>eep</t>
+  </si>
+  <si>
+    <t>Slow Release</t>
+  </si>
+  <si>
+    <t>Nitrification Inhibitor</t>
+  </si>
+  <si>
+    <t>did_you_burn_residue</t>
+  </si>
+  <si>
+    <t>"01/01/1999"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,7 +518,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF2A2C2C"/>
       <name val="Arial"/>
@@ -514,7 +540,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -561,14 +587,14 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -576,6 +602,11 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1076,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B479D4AE-FA7D-CA44-BF82-B5408D6E0BCF}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1107,7 +1138,7 @@
     </row>
     <row r="3" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B3" s="11"/>
     </row>
@@ -1115,176 +1146,200 @@
       <c r="A4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>1</v>
+      <c r="B4" s="9" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>129</v>
+        <v>125</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="12">
-        <v>43</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B6" s="10"/>
     </row>
     <row r="7" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="12">
-        <v>10</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="B7" s="10"/>
     </row>
     <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>86</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>121</v>
+        <v>70</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="12"/>
     </row>
     <row r="13" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>102</v>
+        <v>73</v>
+      </c>
+      <c r="B13" s="12">
+        <v>2000</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>3</v>
+        <v>74</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="B20" s="12">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B21" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>100</v>
+        <v>82</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="10" t="s">
+    <row r="26" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+    <row r="28" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>125</v>
+    </row>
+    <row r="29" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1294,54 +1349,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Choose" prompt="Make a choice" xr:uid="{C3AD2C11-A234-5E47-8591-D75A01B1DC7E}">
           <x14:formula1>
             <xm:f>yesno!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B4 B16 B18</xm:sqref>
+          <xm:sqref>B19 B17 B4:B5 B29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Choose a crop" error="Choose a crop" promptTitle="Crop" prompt="choose crop" xr:uid="{97E5F41B-79F3-664A-BF6C-E828031A2348}">
           <x14:formula1>
             <xm:f>crops!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C662B32F-7BC6-3241-AB1A-835972BD7A98}">
           <x14:formula1>
             <xm:f>'pre1980'!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B8</xm:sqref>
+          <xm:sqref>B9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CCDB6A5C-E9F5-6245-BC32-084800935ED7}">
           <x14:formula1>
             <xm:f>'yr80'!$A$1:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
+          <xm:sqref>B10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7694CF7-8399-CC4F-8262-DA676248F9C3}">
           <x14:formula1>
             <xm:f>tillage!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
+          <xm:sqref>B11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1876C627-C0B8-8143-B7E3-48E6C3FB7181}">
           <x14:formula1>
             <xm:f>binary!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B13</xm:sqref>
+          <xm:sqref>B14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{820F4AB1-A385-A643-B9BE-3195C74F83D9}">
           <x14:formula1>
             <xm:f>tillagetype!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B22</xm:sqref>
+          <xm:sqref>B23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{62EC0EF5-D38F-C34F-A670-E8811702E4E5}">
           <x14:formula1>
             <xm:f>napplicationtype!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B24</xm:sqref>
+          <xm:sqref>B25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FC890307-F2BA-924E-BE04-0B6F11539892}">
+          <x14:formula1>
+            <xm:f>napplicationmethod!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B27</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D378460A-E4DD-C547-9419-7FB5190463BC}">
+          <x14:formula1>
+            <xm:f>eep!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1350,6 +1417,74 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E3703A-3DA3-1343-819D-167B46A84488}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D564B03-164D-154C-8A71-3191222F40FA}">
   <dimension ref="A1:A9"/>
   <sheetViews>
@@ -1364,47 +1499,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1413,7 +1548,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3C9515-4904-A94F-84AB-7579174EE5B8}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D6820C7-4691-BF4C-99FC-BAF63356F37A}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1427,17 +1602,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1447,12 +1622,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB5D2F5-09C0-5D41-B791-F567343A980B}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BF609B-1F57-E245-805C-345CE448249A}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1461,22 +1664,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1485,7 +1688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1425D712-AC41-924C-A9AE-3E51B7EDF505}">
   <dimension ref="A1:A9"/>
   <sheetViews>
@@ -1496,47 +1699,47 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1545,12 +1748,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DA19AE-C34D-9342-969B-07301959E3E1}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1566,14 +1769,16 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="7" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A963F5CA-9031-6442-8BE3-8F7DE6802028}">
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -1863,7 +2068,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF27384-76BF-B542-A9B2-05B92B0EBBB8}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1993,7 +2198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5DA86C-720F-E54A-B3B0-93F1CA124C2E}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -2084,7 +2289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DD3F6A-7E39-6C4F-A01B-DC7DE0459EB8}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2107,72 +2312,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E3703A-3DA3-1343-819D-167B46A84488}">
-  <dimension ref="A1:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Testing of API for success
</commit_message>
<xml_diff>
--- a/template_v1.xlsx
+++ b/template_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpollard/projects/comet/COMET-Farm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EBC989-FCA8-7D4A-A30F-8010A512DEFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21B9FE2-E16C-5149-A6D3-BB056FB7385B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6980" yWindow="460" windowWidth="26620" windowHeight="20540" xr2:uid="{5384504D-6727-334D-8532-C0C118A2956A}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="139">
   <si>
     <t>Yes</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>Di-Ammonium Phosphate</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
   <si>
     <t>id</t>
@@ -1109,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B479D4AE-FA7D-CA44-BF82-B5408D6E0BCF}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1138,7 +1141,7 @@
     </row>
     <row r="3" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B3" s="11"/>
     </row>
@@ -1147,15 +1150,15 @@
         <v>65</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1166,13 +1169,13 @@
     </row>
     <row r="7" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B7" s="10"/>
     </row>
     <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" s="10"/>
     </row>
@@ -1204,7 +1207,9 @@
       <c r="A12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="12" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="13" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -1235,7 +1240,7 @@
         <v>76</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1251,7 +1256,7 @@
         <v>78</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1283,7 +1288,7 @@
         <v>82</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1299,7 +1304,7 @@
         <v>84</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1312,7 +1317,7 @@
     </row>
     <row r="26" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B26" s="12">
         <v>100</v>
@@ -1320,23 +1325,23 @@
     </row>
     <row r="27" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>1</v>
@@ -1560,27 +1565,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1633,17 +1638,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1770,7 +1775,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>